<commit_message>
Before changing vmixclient to pointer
</commit_message>
<xml_diff>
--- a/responses.xlsx
+++ b/responses.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Responses" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="91">
   <si>
     <t xml:space="preserve">Button</t>
   </si>
@@ -75,6 +75,9 @@
     <t xml:space="preserve">Thanks be to God. Alleluia</t>
   </si>
   <si>
+    <t xml:space="preserve">Is this working?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Affirmation of Faith</t>
   </si>
   <si>
@@ -283,6 +286,9 @@
   </si>
   <si>
     <t xml:space="preserve">dumpVars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merge Input=1</t>
   </si>
   <si>
     <t xml:space="preserve">Fader</t>
@@ -657,10 +663,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -669,6 +675,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -893,6 +900,20 @@
       </c>
       <c r="D16" s="0" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -925,23 +946,24 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="23.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="31.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="37.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -986,72 +1008,72 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1083,35 +1105,36 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="22.89"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="11.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="14.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1131,68 +1154,68 @@
         <v>29</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I2" s="11"/>
       <c r="J2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J3" s="17"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I4" s="22"/>
       <c r="J4" s="23"/>
@@ -1221,37 +1244,37 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J6" s="17"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I7" s="22"/>
       <c r="J7" s="23"/>
@@ -1278,33 +1301,33 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C9" s="0"/>
       <c r="D9" s="13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J9" s="17"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C10" s="0"/>
       <c r="D10" s="19" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F10" s="22"/>
       <c r="G10" s="22"/>
@@ -1332,29 +1355,29 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J12" s="17"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B13" s="13"/>
       <c r="C13" s="0"/>
       <c r="D13" s="19" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
@@ -1382,28 +1405,28 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15" s="0"/>
       <c r="D15" s="13" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J15" s="17"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B16" s="0"/>
       <c r="C16" s="19"/>
       <c r="D16" s="19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
@@ -1429,22 +1452,22 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B18" s="0"/>
       <c r="D18" s="13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J18" s="17"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B19" s="25"/>
       <c r="C19" s="19"/>
       <c r="D19" s="19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E19" s="25"/>
       <c r="F19" s="22"/>
@@ -1469,7 +1492,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B21" s="0"/>
       <c r="D21" s="0"/>
@@ -1478,7 +1501,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B22" s="0"/>
       <c r="C22" s="19"/>
@@ -1506,14 +1529,14 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D24" s="13"/>
       <c r="J24" s="17"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B25" s="25"/>
       <c r="C25" s="19"/>
@@ -1541,7 +1564,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D27" s="0"/>
       <c r="E27" s="0"/>
@@ -1549,7 +1572,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
@@ -1577,13 +1600,13 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J30" s="17"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
@@ -1611,14 +1634,14 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D33" s="0"/>
       <c r="J33" s="17"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="19"/>
@@ -1646,14 +1669,14 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D36" s="0"/>
       <c r="J36" s="17"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B37" s="19"/>
       <c r="C37" s="19"/>
@@ -1681,13 +1704,13 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J39" s="17"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B40" s="19"/>
       <c r="C40" s="19"/>
@@ -1715,13 +1738,13 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J42" s="17"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B43" s="19"/>
       <c r="C43" s="19"/>
@@ -1749,10 +1772,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1761,6 +1784,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="34.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="26" width="21.78"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="5" style="26" width="11.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="258" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1768,10 +1792,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1779,7 +1803,7 @@
         <v>56</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1787,7 +1811,7 @@
         <v>48</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1795,7 +1819,7 @@
         <v>51</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1803,7 +1827,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1811,7 +1835,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1819,7 +1843,15 @@
         <v>98</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>85</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1845,10 +1877,13 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
@@ -1913,7 +1948,7 @@
         <v>55</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1921,7 +1956,7 @@
         <v>56</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changing activator actions to string slice
</commit_message>
<xml_diff>
--- a/responses.xlsx
+++ b/responses.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Responses" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="95">
   <si>
     <t xml:space="preserve">Button</t>
   </si>
@@ -246,9 +246,15 @@
     <t xml:space="preserve">yellow: 40</t>
   </si>
   <si>
+    <t xml:space="preserve">red: 0</t>
+  </si>
+  <si>
     <t xml:space="preserve">red: 66</t>
   </si>
   <si>
+    <t xml:space="preserve">green: 0</t>
+  </si>
+  <si>
     <t xml:space="preserve">off: 66</t>
   </si>
   <si>
@@ -288,7 +294,33 @@
     <t xml:space="preserve">dumpVars</t>
   </si>
   <si>
-    <t xml:space="preserve">Merge Input=1</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Merge Input=2
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">leds green 0
+leds yellow 8,9,10</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">leds red 0
+leds yellow 1
+Merge Input=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leds off 49</t>
   </si>
   <si>
     <t xml:space="preserve">Fader</t>
@@ -308,7 +340,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -342,6 +374,11 @@
       <name val="DejaVu Sans"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -469,7 +506,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -584,6 +621,14 @@
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -665,8 +710,8 @@
   </sheetPr>
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1095,7 +1140,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1339,7 +1384,9 @@
       <c r="A11" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="24"/>
+      <c r="B11" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8" t="n">
         <v>6</v>
@@ -1357,10 +1404,12 @@
       <c r="A12" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="13"/>
+      <c r="B12" s="13" t="s">
+        <v>73</v>
+      </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>69</v>
@@ -1371,10 +1420,12 @@
       <c r="A13" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="13"/>
+      <c r="B13" s="13" t="s">
+        <v>75</v>
+      </c>
       <c r="C13" s="0"/>
       <c r="D13" s="19" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>72</v>
@@ -1409,7 +1460,7 @@
       </c>
       <c r="B15" s="0"/>
       <c r="D15" s="13" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>69</v>
@@ -1423,7 +1474,7 @@
       <c r="B16" s="0"/>
       <c r="C16" s="19"/>
       <c r="D16" s="19" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>72</v>
@@ -1456,7 +1507,7 @@
       </c>
       <c r="B18" s="0"/>
       <c r="D18" s="13" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="J18" s="17"/>
     </row>
@@ -1467,7 +1518,7 @@
       <c r="B19" s="25"/>
       <c r="C19" s="19"/>
       <c r="D19" s="19" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E19" s="25"/>
       <c r="F19" s="22"/>
@@ -1772,10 +1823,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1792,10 +1843,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1803,7 +1854,7 @@
         <v>56</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1811,7 +1862,7 @@
         <v>48</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1819,7 +1870,7 @@
         <v>51</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1827,7 +1878,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1835,7 +1886,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1843,16 +1894,28 @@
         <v>98</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="26" t="n">
         <v>0</v>
       </c>
-      <c r="B8" s="27" t="s">
-        <v>87</v>
-      </c>
+      <c r="B8" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="26" t="n">
+        <v>49</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1883,7 +1946,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
@@ -1948,7 +2011,7 @@
         <v>55</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1956,7 +2019,7 @@
         <v>56</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Activator actions changed to slice
</commit_message>
<xml_diff>
--- a/responses.xlsx
+++ b/responses.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="96">
   <si>
     <t xml:space="preserve">Button</t>
   </si>
@@ -159,7 +159,8 @@
     <t xml:space="preserve">Action On</t>
   </si>
   <si>
-    <t xml:space="preserve">red: 1</t>
+    <t xml:space="preserve">red: 1
+green: 2</t>
   </si>
   <si>
     <t xml:space="preserve">yellow: 49,50,51,52</t>
@@ -183,7 +184,7 @@
     <t xml:space="preserve">Action Off</t>
   </si>
   <si>
-    <t xml:space="preserve">off: 1</t>
+    <t xml:space="preserve">off: 1,2</t>
   </si>
   <si>
     <t xml:space="preserve">off: 49,50,51,52</t>
@@ -246,13 +247,7 @@
     <t xml:space="preserve">yellow: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">red: 0</t>
-  </si>
-  <si>
     <t xml:space="preserve">red: 66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">green: 0</t>
   </si>
   <si>
     <t xml:space="preserve">off: 66</t>
@@ -321,6 +316,15 @@
   </si>
   <si>
     <t xml:space="preserve">leds off 49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merge Input=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merge Input=2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merge Input=3</t>
   </si>
   <si>
     <t xml:space="preserve">Fader</t>
@@ -560,7 +564,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -711,7 +715,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1140,7 +1144,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1210,7 +1214,7 @@
       <c r="I2" s="11"/>
       <c r="J2" s="10"/>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
         <v>43</v>
       </c>
@@ -1384,9 +1388,7 @@
       <c r="A11" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="24" t="n">
-        <v>1</v>
-      </c>
+      <c r="B11" s="24"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8" t="n">
         <v>6</v>
@@ -1404,12 +1406,10 @@
       <c r="A12" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>73</v>
-      </c>
+      <c r="B12" s="13"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>69</v>
@@ -1420,12 +1420,10 @@
       <c r="A13" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>75</v>
-      </c>
+      <c r="B13" s="13"/>
       <c r="C13" s="0"/>
       <c r="D13" s="19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>72</v>
@@ -1460,7 +1458,7 @@
       </c>
       <c r="B15" s="0"/>
       <c r="D15" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>69</v>
@@ -1474,7 +1472,7 @@
       <c r="B16" s="0"/>
       <c r="C16" s="19"/>
       <c r="D16" s="19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>72</v>
@@ -1507,7 +1505,7 @@
       </c>
       <c r="B18" s="0"/>
       <c r="D18" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J18" s="17"/>
     </row>
@@ -1518,7 +1516,7 @@
       <c r="B19" s="25"/>
       <c r="C19" s="19"/>
       <c r="D19" s="19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E19" s="25"/>
       <c r="F19" s="22"/>
@@ -1823,10 +1821,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1843,10 +1841,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1854,7 +1852,7 @@
         <v>56</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1862,7 +1860,7 @@
         <v>48</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1870,7 +1868,7 @@
         <v>51</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1878,7 +1876,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1886,7 +1884,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1894,7 +1892,7 @@
         <v>98</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1902,10 +1900,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1913,9 +1911,35 @@
         <v>49</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="26" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="26" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="26" t="n">
+        <v>3</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1946,7 +1970,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
@@ -2011,7 +2035,7 @@
         <v>55</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2019,7 +2043,7 @@
         <v>56</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>